<commit_message>
Add aboriginal police services
</commit_message>
<xml_diff>
--- a/sources/police_stations/sources.xlsx
+++ b/sources/police_stations/sources.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
   <si>
     <t>Province</t>
   </si>
@@ -214,6 +214,21 @@
   </si>
   <si>
     <t>Needs scraping</t>
+  </si>
+  <si>
+    <t>https://www.apscops.org/detachments/</t>
+  </si>
+  <si>
+    <t>Anishinabek</t>
+  </si>
+  <si>
+    <t>http://www.naps.ca/index.php?option=com_content&amp;view=article&amp;id=64&amp;Itemid=34</t>
+  </si>
+  <si>
+    <t>Nishnawbe-Aski</t>
+  </si>
+  <si>
+    <t>PDF</t>
   </si>
 </sst>
 </file>
@@ -534,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,47 +853,47 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,13 +901,16 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -900,16 +918,16 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,38 +935,69 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>60</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>63</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E26" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1"/>
+    <hyperlink ref="C26" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>